<commit_message>
ng: add tas sokoto forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/nov 2024/Sokoto & Kaduna/ng_lf_tas_2411_2_fts_sk_kd.xlsx
+++ b/LF/TAS/Nigeria/2024/nov 2024/Sokoto & Kaduna/ng_lf_tas_2411_2_fts_sk_kd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\oct_2024\Yobe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\nov 2024\Sokoto &amp; Kaduna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499A225-3C22-4088-939F-D35E9B8C33E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4D70A8-6054-4895-8E56-DE32AEE4702C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="191">
   <si>
     <t>type</t>
   </si>
@@ -559,13 +559,58 @@
     <t>Select the community</t>
   </si>
   <si>
-    <t>ng_lf_tas_2410_2_fts_yb</t>
-  </si>
-  <si>
-    <t>ng_tas_fts_2410_yb</t>
-  </si>
-  <si>
-    <t>(Octobre 2024) Yobe - 2. TAS1 LF FTS Form</t>
+    <t>ng_lf_tas_2411_2_fts_yb</t>
+  </si>
+  <si>
+    <t>(Novembre 2024) Sokoto &amp; Kaduna - 2. TAS1 LF FTS Form</t>
+  </si>
+  <si>
+    <t>ng_tas_fts_2411_sk</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_1</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_2</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_3</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_4</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_5</t>
+  </si>
+  <si>
+    <t>bind::db_get</t>
+  </si>
+  <si>
+    <t>col_1</t>
+  </si>
+  <si>
+    <t>col_2</t>
+  </si>
+  <si>
+    <t>col_3</t>
+  </si>
+  <si>
+    <t>col_4</t>
+  </si>
+  <si>
+    <t>col_5</t>
+  </si>
+  <si>
+    <t>${d_eu}</t>
+  </si>
+  <si>
+    <t>${d_district}</t>
+  </si>
+  <si>
+    <t>${d_community}</t>
+  </si>
+  <si>
+    <t>${d_cluster_name}</t>
   </si>
 </sst>
 </file>
@@ -633,7 +678,7 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1125,13 +1170,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1149,10 +1194,14 @@
     <col min="11" max="11" width="35.375" style="27" customWidth="1"/>
     <col min="12" max="12" width="13.875" style="27" customWidth="1"/>
     <col min="13" max="13" width="36.625" style="27" customWidth="1"/>
-    <col min="14" max="16384" width="11" style="27"/>
+    <col min="14" max="14" width="11" style="27"/>
+    <col min="15" max="15" width="17.75" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="22.125" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.75" style="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="37.5">
+    <row r="1" spans="1:21" s="16" customFormat="1" ht="37.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1198,8 +1247,26 @@
       <c r="O1" s="41" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="16" customFormat="1" ht="47.25">
+      <c r="P1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="16" customFormat="1" ht="47.25">
       <c r="A2" s="29" t="s">
         <v>134</v>
       </c>
@@ -1224,7 +1291,7 @@
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
     </row>
-    <row r="3" spans="1:15" s="16" customFormat="1">
+    <row r="3" spans="1:21" s="16" customFormat="1">
       <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
@@ -1242,8 +1309,11 @@
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39"/>
-    </row>
-    <row r="4" spans="1:15" s="16" customFormat="1">
+      <c r="U3" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="16" customFormat="1">
       <c r="A4" s="16" t="s">
         <v>32</v>
       </c>
@@ -1264,8 +1334,14 @@
       </c>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1">
+      <c r="P4" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="16" customFormat="1">
       <c r="A5" s="16" t="s">
         <v>32</v>
       </c>
@@ -1286,8 +1362,14 @@
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
-    </row>
-    <row r="6" spans="1:15" s="16" customFormat="1">
+      <c r="Q5" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="16" customFormat="1">
       <c r="A6" s="16" t="s">
         <v>32</v>
       </c>
@@ -1308,8 +1390,14 @@
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
-    </row>
-    <row r="7" spans="1:15" s="16" customFormat="1">
+      <c r="R6" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="16" customFormat="1">
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
@@ -1330,8 +1418,14 @@
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
-    </row>
-    <row r="8" spans="1:15" s="16" customFormat="1" ht="31.5">
+      <c r="S7" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="16" customFormat="1" ht="31.5">
       <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1447,7 @@
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
     </row>
-    <row r="9" spans="1:15" s="16" customFormat="1">
+    <row r="9" spans="1:21" s="16" customFormat="1">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -1374,12 +1468,12 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:15" s="16" customFormat="1">
+    <row r="10" spans="1:21" s="16" customFormat="1">
       <c r="A10" s="17" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>104</v>
@@ -1399,7 +1493,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="16" customFormat="1">
+    <row r="11" spans="1:21" s="16" customFormat="1">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1420,7 +1514,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:15" s="16" customFormat="1">
+    <row r="12" spans="1:21" s="16" customFormat="1">
       <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
@@ -1441,7 +1535,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:15" s="16" customFormat="1">
+    <row r="13" spans="1:21" s="16" customFormat="1">
       <c r="A13" s="10" t="s">
         <v>102</v>
       </c>
@@ -1464,7 +1558,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:15" s="16" customFormat="1" ht="31.5">
+    <row r="14" spans="1:21" s="16" customFormat="1" ht="31.5">
       <c r="A14" s="29" t="s">
         <v>150</v>
       </c>
@@ -1493,7 +1587,7 @@
       <c r="L14" s="30"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="1:15" s="16" customFormat="1">
+    <row r="15" spans="1:21" s="16" customFormat="1">
       <c r="A15" s="29" t="s">
         <v>21</v>
       </c>
@@ -1518,7 +1612,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:15" s="16" customFormat="1" ht="31.5">
+    <row r="16" spans="1:21" s="16" customFormat="1" ht="31.5">
       <c r="A16" s="29" t="s">
         <v>25</v>
       </c>
@@ -1980,6 +2074,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3670,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3698,7 +3793,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>173</v>

</xml_diff>